<commit_message>
Finished parts list for electronics box frame
</commit_message>
<xml_diff>
--- a/Stuecklisten/Stueckliste_Elektrobox_Rahmen.xlsx
+++ b/Stuecklisten/Stueckliste_Elektrobox_Rahmen.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bulme-my.sharepoint.com/personal/florian_kunz_ms_bulme_at/Documents/HTL Bulme/SJ202526/SPL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HTL_Bulme\SPL_Project_Watermelon\CandyMachine_Watermelon\Stuecklisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{C21F3410-6AA2-4450-8098-F360CD8927B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E4C74FF-12A4-4C08-916C-31F4F8242BB3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBDFCA43-FBEF-475D-AD4D-AC7413B151D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{797F69E5-6349-40C8-ABC7-0C572E2B2F92}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Anzahl</t>
   </si>
@@ -90,6 +90,39 @@
   </si>
   <si>
     <t>8x 15x15x100mm</t>
+  </si>
+  <si>
+    <t>9x hexagon head bolt</t>
+  </si>
+  <si>
+    <t>MakerBeamXL - 15x15mm 50 pieces T-slot nuts for MakerBeamXL</t>
+  </si>
+  <si>
+    <t>https://www.makerbeam.com/t-slot-nuts-for-makerbeamxl-50p.html</t>
+  </si>
+  <si>
+    <t>OpenBeam - 15x15mm 100 pieces, M3, 6mm, button head socket bolt for 15x15mm</t>
+  </si>
+  <si>
+    <t>https://www.makerbeam.com/openbeam-button-head-socket-bolt-6mm-100p-for-open.html</t>
+  </si>
+  <si>
+    <t>28x button head socket bolt</t>
+  </si>
+  <si>
+    <t>https://at.rs-online.com/web/p/maschinenschrauben/0553396?cm_mmc=AT-PLA-DS3A-_-google-_-CSS_AT_DE_Pmax_Test-_--_-553396&amp;matchtype=&amp;&amp;gclsrc=aw.ds&amp;gad_source=1&amp;gad_campaignid=20298205821&amp;gbraid=0AAAAADkeWNOMk3njhx3G3UuxBKKpXpIzU&amp;gclid=CjwKCAiA4KfLBhB0EiwAUY7GAVIHP6yNCVoEI38KaxgYXcveDheFoWhoKTnW8EtL1ZMtSL_iyDy5LhoCUXQQAvD_BwE</t>
+  </si>
+  <si>
+    <t>553-396</t>
+  </si>
+  <si>
+    <t>32x T-slot nuts</t>
+  </si>
+  <si>
+    <t>4x Senkkopfschraube</t>
+  </si>
+  <si>
+    <t>RS PRO Senkkopf Pozi Schrauben verzinkt, M3 x 6.0mm Stahl (100 Stk)</t>
   </si>
 </sst>
 </file>
@@ -137,10 +170,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -476,15 +512,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{873408D1-FEA1-4C01-9395-0C80F48BC176}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="53.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -601,6 +640,81 @@
       <c r="F5" s="1">
         <f>A5*C5</f>
         <v>7.35</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1">
+        <v>17.5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6">
+        <v>103295</v>
+      </c>
+      <c r="F6" s="1">
+        <f>A6*C6</f>
+        <v>17.5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5.98</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7">
+        <v>100933</v>
+      </c>
+      <c r="F7" s="1">
+        <f>A7*C7</f>
+        <v>5.98</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4.57</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="1">
+        <f>A8*C8</f>
+        <v>4.57</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -609,6 +723,9 @@
     <hyperlink ref="B3" r:id="rId2" xr:uid="{4B87E657-81C3-438E-A0E8-9BB0929454E9}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{A97136B6-AF32-46AF-9029-6A45E767EFD4}"/>
     <hyperlink ref="B5" r:id="rId4" xr:uid="{42C93B06-26D3-4FBF-B0AD-983BE0B36243}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{9CE5EA8C-B8AC-4045-AA18-8B5C4E0D3304}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{52A401C4-EDC4-45A2-8237-D23D79BA72BC}"/>
+    <hyperlink ref="B8" r:id="rId7" display="https://at.rs-online.com/web/p/maschinenschrauben/0553396?cm_mmc=AT-PLA-DS3A-_-google-_-CSS_AT_DE_Pmax_Test-_--_-553396&amp;matchtype=&amp;&amp;gclsrc=aw.ds&amp;gad_source=1&amp;gad_campaignid=20298205821&amp;gbraid=0AAAAADkeWNOMk3njhx3G3UuxBKKpXpIzU&amp;gclid=CjwKCAiA4KfLBhB0EiwAUY7GAVIHP6yNCVoEI38KaxgYXcveDheFoWhoKTnW8EtL1ZMtSL_iyDy5LhoCUXQQAvD_BwE" xr:uid="{0804A52B-89F5-4EBA-B3F0-A58D18CE9F95}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>